<commit_message>
Added run for config -Min1-Max<=2 all countries
</commit_message>
<xml_diff>
--- a/csv_out/new2/country_classification_comparison_using_grouped_words_full_updated.xlsx
+++ b/csv_out/new2/country_classification_comparison_using_grouped_words_full_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\IMF_VE_News\csv_out\new2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4683BEF-572C-4F00-8C83-19EE24F39DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55AC052-0FF3-43AC-80D1-8A5EB9C1B409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country_classification_comparis" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>All Other Sentiments</t>
   </si>
@@ -88,9 +88,6 @@
     <t>First 5 Crisis Countries (Title + Full Document) - Limited mentions of other countries</t>
   </si>
   <si>
-    <t>Only top_n countries (and tied) alowed</t>
-  </si>
-  <si>
     <t>Basic Topic Discrimination</t>
   </si>
   <si>
@@ -128,6 +125,15 @@
   </si>
   <si>
     <t>Overall Index Evaluation (Full Table) based on "Grouped Search Words Final"</t>
+  </si>
+  <si>
+    <t>Min1_Top1_AllCountry</t>
+  </si>
+  <si>
+    <t>Min3_Top1_AllCountry</t>
+  </si>
+  <si>
+    <t>Only top_n countries (and tied) alowed - First Five Countries</t>
   </si>
 </sst>
 </file>
@@ -1019,9 +1025,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG31"/>
+  <dimension ref="A1:AG35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1053,7 +1061,7 @@
   <sheetData>
     <row r="1" spans="1:33" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1912,7 +1920,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="7">
         <v>0.55147058823529405</v>
@@ -2007,7 +2015,7 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="7">
         <v>0.62992125984251901</v>
@@ -2102,7 +2110,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="7">
         <v>0.47297297297297303</v>
@@ -2265,7 +2273,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="7">
         <v>8.3333333333333301E-2</v>
@@ -2360,7 +2368,7 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="7">
         <v>0.38461538461538403</v>
@@ -2455,7 +2463,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="7">
         <v>0.116279069767441</v>
@@ -2550,7 +2558,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="7">
         <v>0.60747663551401798</v>
@@ -2677,7 +2685,7 @@
     </row>
     <row r="25" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
@@ -2713,7 +2721,7 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="7">
         <v>0.66666666666666596</v>
@@ -2808,7 +2816,7 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="7">
         <v>0.49180327868852403</v>
@@ -2935,7 +2943,7 @@
     </row>
     <row r="29" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
@@ -2971,7 +2979,7 @@
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="7">
         <v>0.547445255474452</v>
@@ -3066,7 +3074,7 @@
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="7">
         <v>0.56390977443609003</v>
@@ -3158,6 +3166,198 @@
       <c r="AF31" s="8">
         <v>0.8</v>
       </c>
+    </row>
+    <row r="34" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>0.47560975609756101</v>
+      </c>
+      <c r="D34">
+        <v>0.185714285714285</v>
+      </c>
+      <c r="E34">
+        <v>0.78</v>
+      </c>
+      <c r="F34">
+        <v>0.49757281553397997</v>
+      </c>
+      <c r="G34">
+        <v>0.19339622641509399</v>
+      </c>
+      <c r="H34">
+        <v>0.82</v>
+      </c>
+      <c r="I34">
+        <v>0.51094890510948898</v>
+      </c>
+      <c r="J34">
+        <v>0.199052132701421</v>
+      </c>
+      <c r="K34">
+        <v>0.84</v>
+      </c>
+      <c r="L34">
+        <v>0.47706422018348599</v>
+      </c>
+      <c r="M34">
+        <v>0.168284789644012</v>
+      </c>
+      <c r="N34">
+        <v>0.88135593220338904</v>
+      </c>
+      <c r="O34">
+        <v>0.418454935622317</v>
+      </c>
+      <c r="P34">
+        <v>0.14233576642335699</v>
+      </c>
+      <c r="Q34">
+        <v>0.8125</v>
+      </c>
+      <c r="R34">
+        <v>0.42857142857142799</v>
+      </c>
+      <c r="S34">
+        <v>0.15207373271889399</v>
+      </c>
+      <c r="T34">
+        <v>0.78571428571428503</v>
+      </c>
+      <c r="U34">
+        <v>0.53738317757009302</v>
+      </c>
+      <c r="V34">
+        <v>0.20535714285714199</v>
+      </c>
+      <c r="W34">
+        <v>0.90196078431372495</v>
+      </c>
+      <c r="X34">
+        <v>0.51229508196721296</v>
+      </c>
+      <c r="Y34">
+        <v>0.19841269841269801</v>
+      </c>
+      <c r="Z34">
+        <v>0.84745762711864303</v>
+      </c>
+      <c r="AA34">
+        <v>0.49118387909319899</v>
+      </c>
+      <c r="AB34">
+        <v>0.194029850746268</v>
+      </c>
+      <c r="AC34">
+        <v>0.79591836734693799</v>
+      </c>
+      <c r="AD34">
+        <v>0.48625792811839302</v>
+      </c>
+      <c r="AE34">
+        <v>0.176245210727969</v>
+      </c>
+      <c r="AF34">
+        <v>0.86792452830188604</v>
+      </c>
+      <c r="AG34"/>
+    </row>
+    <row r="35" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <v>0.29255319148936099</v>
+      </c>
+      <c r="D35">
+        <v>0.16176470588235201</v>
+      </c>
+      <c r="E35">
+        <v>0.36666666666666597</v>
+      </c>
+      <c r="F35">
+        <v>0.25280898876404401</v>
+      </c>
+      <c r="G35">
+        <v>0.13636363636363599</v>
+      </c>
+      <c r="H35">
+        <v>0.32142857142857101</v>
+      </c>
+      <c r="I35">
+        <v>0.39408866995073799</v>
+      </c>
+      <c r="J35">
+        <v>0.22535211267605601</v>
+      </c>
+      <c r="K35">
+        <v>0.48484848484848397</v>
+      </c>
+      <c r="L35">
+        <v>0.39432176656151402</v>
+      </c>
+      <c r="M35">
+        <v>0.15151515151515099</v>
+      </c>
+      <c r="N35">
+        <v>0.65789473684210498</v>
+      </c>
+      <c r="O35">
+        <v>0.36170212765957399</v>
+      </c>
+      <c r="P35">
+        <v>0.153153153153153</v>
+      </c>
+      <c r="Q35">
+        <v>0.54838709677419295</v>
+      </c>
+      <c r="R35">
+        <v>0.34574468085106302</v>
+      </c>
+      <c r="S35">
+        <v>0.180555555555555</v>
+      </c>
+      <c r="T35">
+        <v>0.44827586206896503</v>
+      </c>
+      <c r="U35">
+        <v>0.34403669724770602</v>
+      </c>
+      <c r="V35">
+        <v>0.159574468085106</v>
+      </c>
+      <c r="W35">
+        <v>0.483870967741935</v>
+      </c>
+      <c r="X35">
+        <v>0.30232558139534799</v>
+      </c>
+      <c r="Y35">
+        <v>0.14285714285714199</v>
+      </c>
+      <c r="Z35">
+        <v>0.41935483870967699</v>
+      </c>
+      <c r="AA35">
+        <v>0.28985507246376802</v>
+      </c>
+      <c r="AB35">
+        <v>0.13793103448275801</v>
+      </c>
+      <c r="AC35">
+        <v>0.4</v>
+      </c>
+      <c r="AD35">
+        <v>0.28985507246376802</v>
+      </c>
+      <c r="AE35">
+        <v>0.13186813186813101</v>
+      </c>
+      <c r="AF35">
+        <v>0.41379310344827502</v>
+      </c>
+      <c r="AG35"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>